<commit_message>
The second day sprint backlog
Committed today because we had to move githubs
</commit_message>
<xml_diff>
--- a/Sprint 1/Sprint_Backlog/Sprint backlog.xlsx
+++ b/Sprint 1/Sprint_Backlog/Sprint backlog.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7305F8-E4F1-4493-A80E-2F9BCF7D4975}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="67">
   <si>
     <t>Agile Group 9 - Sprint 1</t>
   </si>
@@ -39,18 +48,18 @@
   <si>
     <r>
       <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="11.0"/>
       </rPr>
       <t>Goal</t>
     </r>
     <r>
       <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
       </rPr>
       <t xml:space="preserve">: Demonstrate the ability for researches to curate questionairres and export data from answered ones. </t>
     </r>
@@ -65,6 +74,9 @@
     <t>Calum Parsons</t>
   </si>
   <si>
+    <t>Initial Velocity = 11</t>
+  </si>
+  <si>
     <t>Shanna Balfour</t>
   </si>
   <si>
@@ -94,19 +106,19 @@
   <si>
     <r>
       <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="14.0"/>
       </rPr>
       <t xml:space="preserve">Done? </t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="9.0"/>
       </rPr>
       <t>(DoD)</t>
     </r>
@@ -118,21 +130,95 @@
     <t>As a researcher, I want to be able to add any questionnaires I have designed to my application so that they can get approval</t>
   </si>
   <si>
+    <t>If a created questionairre can be attached to an email then accept</t>
+  </si>
+  <si>
+    <t>Shaun, Tim</t>
+  </si>
+  <si>
     <t>Y/N</t>
   </si>
   <si>
     <t>As a researcher, I want to be able to export data from the questionnaire so that the data can be used for analysis.</t>
   </si>
   <si>
+    <t>All of the questionairre responses can be downloaded in an accessible and easily processible format</t>
+  </si>
+  <si>
+    <t>Shanna</t>
+  </si>
+  <si>
     <t>As a stakeholder, I want participants to only have access to questionnaires so that the rest of the experiment is private and safe</t>
   </si>
   <si>
+    <t>When participants log in, they will only have access to questionnaires on their homepage.</t>
+  </si>
+  <si>
+    <t>Laura + Michael</t>
+  </si>
+  <si>
     <t>As a researcher I want to be able to send questionnaires for participants to fill in so I can collect data from users</t>
   </si>
   <si>
+    <t>Researchers are able to send specific questionnaires to specific participants</t>
+  </si>
+  <si>
+    <t>Gina</t>
+  </si>
+  <si>
     <t>As a researcher, I want the ability to create a questionnaire so that they can be sent to users.</t>
   </si>
   <si>
+    <t>Questionnaires can be designed or processed by the program into its own suitable format</t>
+  </si>
+  <si>
+    <t>Ema, Calum</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Other Tasks:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Not Stories, but still need done</t>
+    </r>
+  </si>
+  <si>
+    <t>Done?</t>
+  </si>
+  <si>
+    <t>Definition of Done:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set up database stuff so we can access it! </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -Meets accessibility guidelines
+-Code has been reviewed
+-Meets acceptance test for story
+-Product Owner accepts story</t>
+  </si>
+  <si>
+    <t>Set up a visual studio c# .net application that works on web</t>
+  </si>
+  <si>
+    <t>Ema + Calum + Timothy</t>
+  </si>
+  <si>
+    <t>Yes! 27/01/21</t>
+  </si>
+  <si>
     <t>Scrum Minutes</t>
   </si>
   <si>
@@ -155,52 +241,154 @@
   </si>
   <si>
     <t>4 :)   3 :|   1 :(</t>
+  </si>
+  <si>
+    <t>4 Spirits, 1 Mock, 2 Beer</t>
+  </si>
+  <si>
+    <t>- Lots of research done into best way to host the software</t>
+  </si>
+  <si>
+    <t>- undertanding visual studio            - feeling lost with where to start</t>
+  </si>
+  <si>
+    <t>-database setup                             -github setup                            - everyone able to work comfortably</t>
+  </si>
+  <si>
+    <t>2 m, 5 b,  1 s</t>
+  </si>
+  <si>
+    <t>-Azure is now up and running our test code</t>
+  </si>
+  <si>
+    <t>-had to change github repo to get it to work</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- need to know how to develope web application with </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>asp.net</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">                                        - find resources for this</t>
+    </r>
+  </si>
+  <si>
+    <t>mocktail (happy) 
+beer (ok still) 
+spirit (getting bad)
+industrial strength (uh oh)</t>
+  </si>
+  <si>
+    <t>M,B,S,I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">daily scrum shouldn't cover the technicalities of work, it should focus on the next steps to solve problems and help keep things moving - technicalities can be done at other times aside from the scrum </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="9">
-    <font>
-      <sz val="10.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
+  </numFmts>
+  <fonts count="15" x14ac:knownFonts="1">
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -208,7 +396,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -223,70 +411,106 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
-    <border/>
+  <borders count="16">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-    </border>
-    <border>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -298,16 +522,26 @@
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -316,100 +550,124 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="42">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="8" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="10" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="13" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -599,304 +857,513 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="30.57"/>
-    <col customWidth="1" min="8" max="8" width="19.0"/>
+    <col min="1" max="1" width="30.5546875" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="B1" s="19"/>
+      <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3">
-      <c r="I3" s="5" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5">
-      <c r="I5" s="5" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6">
-      <c r="I6" s="5" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="I6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7">
-      <c r="I7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="6" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8">
-      <c r="I8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="6" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I9" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="11" t="s">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="14" t="s">
+      <c r="B11" s="26"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="14" t="s">
+      <c r="E11" s="26"/>
+      <c r="F11" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="14" t="s">
+      <c r="G11" s="26"/>
+      <c r="H11" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="J11" s="15" t="s">
+      <c r="I11" s="29" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="C12" s="16"/>
-      <c r="F12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="18"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="19" t="s">
+      <c r="J11" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="H13" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="I13" s="20" t="s">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="32"/>
+    </row>
+    <row r="13" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="J13" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="19" t="s">
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="H14" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="19" t="s">
+      <c r="E13" s="19"/>
+      <c r="F13" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="H15" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="19" t="s">
+      <c r="G13" s="19"/>
+      <c r="H13" s="12">
+        <v>2</v>
+      </c>
+      <c r="I13" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="H16" s="20">
-        <v>2.0</v>
-      </c>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="19" t="s">
+      <c r="J13" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="H17" s="20">
-        <v>3.0</v>
-      </c>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="22"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="24" t="s">
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="41" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="25" t="s">
+      <c r="E14" s="19"/>
+      <c r="F14" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="G14" s="19"/>
+      <c r="H14" s="12">
+        <v>2</v>
+      </c>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+    </row>
+    <row r="15" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="26" t="s">
+      <c r="E15" s="19"/>
+      <c r="F15" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="G21" s="26" t="s">
+      <c r="G15" s="19"/>
+      <c r="H15" s="12">
+        <v>2</v>
+      </c>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+    </row>
+    <row r="16" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="27" t="s">
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="E16" s="19"/>
+      <c r="F16" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="7"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="7"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="7"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="7"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="7"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="7"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="7"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="7"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="12">
+        <v>2</v>
+      </c>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="19"/>
+      <c r="F17" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="19"/>
+      <c r="H17" s="12">
+        <v>3</v>
+      </c>
+      <c r="I17" s="13"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="19"/>
+      <c r="F18" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="I19" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="J19" s="19"/>
+    </row>
+    <row r="20" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A20" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="19"/>
+      <c r="I20" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="J20" s="19"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="19"/>
+      <c r="F21" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+    </row>
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="37"/>
+      <c r="E25" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" s="37"/>
+      <c r="G25" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="H25" s="38"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="23"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="17">
+        <v>44222</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="19"/>
+      <c r="E27" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" s="19"/>
+      <c r="G27" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="H27" s="19"/>
+    </row>
+    <row r="28" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A28" s="17">
+        <v>44223</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="19"/>
+      <c r="E28" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" s="19"/>
+      <c r="G28" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="H28" s="19"/>
+    </row>
+    <row r="29" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="J29" s="19"/>
+    </row>
+    <row r="30" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+    </row>
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+    </row>
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+    </row>
+    <row r="34" spans="9:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="I34" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+    </row>
+    <row r="35" spans="9:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+    </row>
+    <row r="36" spans="9:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
+    </row>
+    <row r="37" spans="9:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="43">
+  <mergeCells count="49">
+    <mergeCell ref="A18:C19"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="D18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I20:J23"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="A15:C15"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
     <mergeCell ref="A11:C12"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="D13:E13"/>
     <mergeCell ref="D11:E12"/>
     <mergeCell ref="F11:G12"/>
     <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
     <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="G27:H27"/>
     <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="C29:D29"/>
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I34:K37"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="I29:J32"/>
     <mergeCell ref="G31:H31"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink ref="G28" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
The third day sprint backlog
Wednesday !
</commit_message>
<xml_diff>
--- a/Sprint 1/Sprint_Backlog/Sprint backlog.xlsx
+++ b/Sprint 1/Sprint_Backlog/Sprint backlog.xlsx
@@ -1,21 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7305F8-E4F1-4493-A80E-2F9BCF7D4975}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
@@ -48,18 +39,18 @@
   <si>
     <r>
       <rPr>
+        <rFont val="Arial"/>
         <b/>
-        <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <sz val="11.0"/>
       </rPr>
       <t>Goal</t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <rFont val="Arial"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <sz val="11.0"/>
       </rPr>
       <t xml:space="preserve">: Demonstrate the ability for researches to curate questionairres and export data from answered ones. </t>
     </r>
@@ -106,19 +97,19 @@
   <si>
     <r>
       <rPr>
+        <rFont val="Arial"/>
         <b/>
-        <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <sz val="14.0"/>
       </rPr>
       <t xml:space="preserve">Done? </t>
     </r>
     <r>
       <rPr>
+        <rFont val="Arial"/>
         <b/>
-        <sz val="9"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <sz val="9.0"/>
       </rPr>
       <t>(DoD)</t>
     </r>
@@ -177,19 +168,19 @@
   <si>
     <r>
       <rPr>
+        <rFont val="Arial"/>
         <b/>
-        <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <sz val="14.0"/>
       </rPr>
       <t>Other Tasks:</t>
     </r>
     <r>
       <rPr>
+        <rFont val="Arial"/>
         <b/>
-        <sz val="9"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <sz val="9.0"/>
       </rPr>
       <t xml:space="preserve"> Not Stories, but still need done</t>
     </r>
@@ -265,23 +256,18 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">- need to know how to develope web application with </t>
     </r>
     <r>
       <rPr>
+        <color rgb="FF1155CC"/>
         <u/>
-        <sz val="10"/>
-        <color rgb="FF1155CC"/>
-        <rFont val="Arial"/>
       </rPr>
       <t>asp.net</t>
     </r>
     <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
+      <rPr/>
       <t xml:space="preserve">                                        - find resources for this</t>
     </r>
   </si>
@@ -301,94 +287,57 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="14.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font/>
+    <font>
+      <sz val="8.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="8"/>
+      <sz val="9.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="12.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="10"/>
       <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF1155CC"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -396,7 +345,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -412,105 +361,69 @@
     </fill>
   </fills>
   <borders count="16">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+    </border>
+    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+    </border>
+    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+    </border>
+    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+    </border>
+    <border>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+    </border>
+    <border>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -522,26 +435,16 @@
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+    </border>
+    <border>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -550,12 +453,8 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+    </border>
+    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -565,109 +464,128 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+    </border>
+    <border>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="42">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="37">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="8" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="9" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="10" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="12" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="13" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="14" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="15" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -857,480 +775,371 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" customWidth="1"/>
-    <col min="8" max="8" width="19" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="30.57"/>
+    <col customWidth="1" min="8" max="8" width="19.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I3" s="4" t="s">
+    <row r="3">
+      <c r="I3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4">
+      <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I5" s="4" t="s">
+    <row r="5">
+      <c r="I5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+    <row r="6">
+      <c r="A6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I7" s="4" t="s">
+    <row r="7">
+      <c r="I7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I8" s="4" t="s">
+    <row r="8">
+      <c r="I8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J8" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I9" s="8" t="s">
+    <row r="9">
+      <c r="I9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J9" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+    <row r="10">
+      <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+    <row r="11">
+      <c r="A11" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="25" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="26"/>
-      <c r="F11" s="29" t="s">
+      <c r="E11" s="13"/>
+      <c r="F11" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="26"/>
-      <c r="H11" s="29" t="s">
+      <c r="G11" s="13"/>
+      <c r="H11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="29" t="s">
+      <c r="I11" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="J11" s="31" t="s">
+      <c r="J11" s="16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="32"/>
-    </row>
-    <row r="13" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
+    <row r="12">
+      <c r="C12" s="17"/>
+      <c r="F12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="19"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="40" t="s">
+      <c r="D13" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="23" t="s">
+      <c r="F13" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="19"/>
-      <c r="H13" s="12">
-        <v>2</v>
-      </c>
-      <c r="I13" s="12" t="s">
+      <c r="H13" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="I13" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="J13" s="12" t="s">
+      <c r="J13" s="21" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
+    <row r="14">
+      <c r="A14" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="41" t="s">
+      <c r="D14" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="19"/>
-      <c r="H14" s="12">
-        <v>2</v>
-      </c>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-    </row>
-    <row r="15" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
+      <c r="H14" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="41" t="s">
+      <c r="D15" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="23" t="s">
+      <c r="F15" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="19"/>
-      <c r="H15" s="12">
-        <v>2</v>
-      </c>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-    </row>
-    <row r="16" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
+      <c r="H15" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="39" t="s">
+      <c r="D16" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="23" t="s">
+      <c r="F16" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G16" s="19"/>
-      <c r="H16" s="12">
-        <v>2</v>
-      </c>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
+      <c r="H16" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="19"/>
-      <c r="F17" s="23" t="s">
+      <c r="F17" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G17" s="19"/>
-      <c r="H17" s="12">
-        <v>3</v>
-      </c>
-      <c r="I17" s="13"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="34" t="s">
+      <c r="H17" s="21">
+        <v>3.0</v>
+      </c>
+      <c r="I17" s="23"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="34" t="s">
+      <c r="D18" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="19"/>
-      <c r="F18" s="34" t="s">
+      <c r="F18" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="I19" s="35" t="s">
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+    </row>
+    <row r="19">
+      <c r="I19" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="J19" s="19"/>
-    </row>
-    <row r="20" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A20" s="23" t="s">
+    </row>
+    <row r="20">
+      <c r="A20" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="23" t="s">
+      <c r="D20" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="19"/>
-      <c r="I20" s="39" t="s">
+      <c r="I20" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="J20" s="19"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="23" t="s">
+    </row>
+    <row r="21">
+      <c r="A21" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="23" t="s">
+      <c r="D21" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="19"/>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-    </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="15" t="s">
+    </row>
+    <row r="24">
+      <c r="A24" s="28" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+    <row r="25">
+      <c r="A25" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="36" t="s">
+      <c r="C25" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="37"/>
-      <c r="E25" s="36" t="s">
+      <c r="D25" s="30"/>
+      <c r="E25" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="F25" s="37"/>
-      <c r="G25" s="36" t="s">
+      <c r="F25" s="30"/>
+      <c r="G25" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="H25" s="38"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="H25" s="31"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="23"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="17">
-        <v>44222</v>
-      </c>
-      <c r="B27" s="11" t="s">
+      <c r="C26" s="7"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="32">
+        <v>44222.0</v>
+      </c>
+      <c r="B27" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="22" t="s">
+      <c r="C27" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="22" t="s">
+      <c r="E27" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="F27" s="19"/>
-      <c r="G27" s="22" t="s">
+      <c r="G27" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="H27" s="19"/>
-    </row>
-    <row r="28" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A28" s="17">
-        <v>44223</v>
-      </c>
-      <c r="B28" s="18" t="s">
+    </row>
+    <row r="28">
+      <c r="A28" s="33">
+        <v>44223.0</v>
+      </c>
+      <c r="B28" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="D28" s="19"/>
-      <c r="E28" s="22" t="s">
+      <c r="E28" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="F28" s="19"/>
-      <c r="G28" s="21" t="s">
+      <c r="G28" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="H28" s="19"/>
-    </row>
-    <row r="29" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="40" t="s">
+    </row>
+    <row r="29">
+      <c r="A29" s="7"/>
+      <c r="I29" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="J29" s="19"/>
-    </row>
-    <row r="30" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+    </row>
+    <row r="30">
+      <c r="A30" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
-    </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
-    </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-    </row>
-    <row r="34" spans="9:11" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="I34" s="20" t="s">
+    </row>
+    <row r="34">
+      <c r="I34" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-    </row>
-    <row r="35" spans="9:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I35" s="19"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="19"/>
-    </row>
-    <row r="36" spans="9:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
-    </row>
-    <row r="37" spans="9:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I37" s="19"/>
-      <c r="J37" s="19"/>
-      <c r="K37" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="A18:C19"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="D18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="I20:J23"/>
-    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I34:K37"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="I29:J32"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A11:C12"/>
+    <mergeCell ref="D11:E12"/>
+    <mergeCell ref="F11:G12"/>
+    <mergeCell ref="H11:H12"/>
     <mergeCell ref="I11:I12"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="D15:E15"/>
@@ -1342,28 +1151,31 @@
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A11:C12"/>
-    <mergeCell ref="D11:E12"/>
-    <mergeCell ref="F11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I34:K37"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="I29:J32"/>
-    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="D18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I20:J23"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="A18:C19"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="C26:D26"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G28" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink r:id="rId1" ref="G28"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
day 4 sprint backlog
</commit_message>
<xml_diff>
--- a/Sprint 1/Sprint_Backlog/Sprint backlog.xlsx
+++ b/Sprint 1/Sprint_Backlog/Sprint backlog.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="72">
   <si>
     <t>Agile Group 9 - Sprint 1</t>
   </si>
@@ -118,13 +118,13 @@
     <t>Accepted?</t>
   </si>
   <si>
-    <t>As a researcher, I want to be able to add any questionnaires I have designed to my application so that they can get approval</t>
+    <t>As a researcher, I want to be able to add any questionnaires I have designed to my ethical application so that they can get approval</t>
   </si>
   <si>
     <t>If a created questionairre can be attached to an email then accept</t>
   </si>
   <si>
-    <t>Shaun, Tim</t>
+    <t>Shaun</t>
   </si>
   <si>
     <t>Y/N</t>
@@ -136,7 +136,7 @@
     <t>All of the questionairre responses can be downloaded in an accessible and easily processible format</t>
   </si>
   <si>
-    <t>Shanna</t>
+    <t>Shanna, Tim (database needs setup first)</t>
   </si>
   <si>
     <t>As a stakeholder, I want participants to only have access to questionnaires so that the rest of the experiment is private and safe</t>
@@ -195,6 +195,9 @@
     <t xml:space="preserve">Set up database stuff so we can access it! </t>
   </si>
   <si>
+    <t>Laura + Timothy</t>
+  </si>
+  <si>
     <t xml:space="preserve"> -Meets accessibility guidelines
 -Code has been reviewed
 -Meets acceptance test for story
@@ -270,6 +273,18 @@
       <rPr/>
       <t xml:space="preserve">                                        - find resources for this</t>
     </r>
+  </si>
+  <si>
+    <t>5 b, 1 s, 1 i</t>
+  </si>
+  <si>
+    <t>- Email code working!                           -MySQL stuff linked and working</t>
+  </si>
+  <si>
+    <t>- overwhelmed (reassigned tasks to help)                                                  - some people can't work until other people have completed their work</t>
+  </si>
+  <si>
+    <t>- get SQL reading                             -make questionairre pages working and branded                                          -add email stuff to send page</t>
   </si>
   <si>
     <t>mocktail (happy) 
@@ -560,14 +575,14 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -939,7 +954,7 @@
       <c r="D14" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="20" t="s">
         <v>30</v>
       </c>
       <c r="H14" s="21">
@@ -1020,54 +1035,54 @@
         <v>43</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="I20" s="27" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="28" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D25" s="30"/>
       <c r="E25" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F25" s="30"/>
       <c r="G25" s="29" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H25" s="31"/>
     </row>
     <row r="26">
       <c r="A26" s="7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C26" s="7"/>
     </row>
@@ -1076,65 +1091,81 @@
         <v>44222.0</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="33">
+      <c r="A28" s="32">
         <v>44223.0</v>
       </c>
-      <c r="B28" s="34" t="s">
-        <v>60</v>
+      <c r="B28" s="20" t="s">
+        <v>61</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="G28" s="35" t="s">
         <v>63</v>
       </c>
+      <c r="G28" s="33" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" s="7"/>
+      <c r="A29" s="34">
+        <v>44224.0</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" s="20" t="s">
+        <v>68</v>
+      </c>
       <c r="I29" s="7" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="7" t="s">
-        <v>65</v>
+      <c r="A30" s="35"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="7" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="34">
       <c r="I34" s="36" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="49">
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
+  <mergeCells count="50">
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
     <mergeCell ref="I34:K37"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="G27:H27"/>
     <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
     <mergeCell ref="C29:D29"/>
-    <mergeCell ref="I29:J32"/>
-    <mergeCell ref="G31:H31"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A11:C12"/>
     <mergeCell ref="D11:E12"/>
@@ -1163,8 +1194,6 @@
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="A18:C19"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="A21:C21"/>
@@ -1172,6 +1201,10 @@
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="G25:H25"/>
     <mergeCell ref="C26:D26"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J32"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="G28"/>

</xml_diff>

<commit_message>
Day 5 Sprint backlog 29/01/21
</commit_message>
<xml_diff>
--- a/Sprint 1/Sprint_Backlog/Sprint backlog.xlsx
+++ b/Sprint 1/Sprint_Backlog/Sprint backlog.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="77">
   <si>
     <t>Agile Group 9 - Sprint 1</t>
   </si>
@@ -154,7 +154,7 @@
     <t>Researchers are able to send specific questionnaires to specific participants</t>
   </si>
   <si>
-    <t>Gina</t>
+    <t>Gina, Shaun</t>
   </si>
   <si>
     <t>As a researcher, I want the ability to create a questionnaire so that they can be sent to users.</t>
@@ -198,6 +198,9 @@
     <t>Laura + Timothy</t>
   </si>
   <si>
+    <t>Yes! 29/01/21</t>
+  </si>
+  <si>
     <t xml:space="preserve"> -Meets accessibility guidelines
 -Code has been reviewed
 -Meets acceptance test for story
@@ -293,10 +296,22 @@
 industrial strength (uh oh)</t>
   </si>
   <si>
+    <t>1 B, 5 S</t>
+  </si>
+  <si>
+    <t>- Yesterday hard, SQL linked now</t>
+  </si>
+  <si>
+    <t>- Feeling Lost                                                  - Left behind                                - File architecture confusing</t>
+  </si>
+  <si>
+    <t>- Get all made pages working                                               - Get some basic SQL function to show off                                                                - Sprint Review</t>
+  </si>
+  <si>
     <t>M,B,S,I</t>
   </si>
   <si>
-    <t xml:space="preserve">daily scrum shouldn't cover the technicalities of work, it should focus on the next steps to solve problems and help keep things moving - technicalities can be done at other times aside from the scrum </t>
+    <t xml:space="preserve">daily scrum shouldn't cover the technicalities of work, it should focus on the next steps and help keep things moving - technicalities can be done at other times aside from the scrum </t>
   </si>
 </sst>
 </file>
@@ -489,7 +504,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -579,9 +594,6 @@
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1037,52 +1049,55 @@
       <c r="D20" s="7" t="s">
         <v>44</v>
       </c>
+      <c r="F20" s="7" t="s">
+        <v>45</v>
+      </c>
       <c r="I20" s="27" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="28" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D25" s="30"/>
       <c r="E25" s="29" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F25" s="30"/>
       <c r="G25" s="29" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H25" s="31"/>
     </row>
     <row r="26">
       <c r="A26" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C26" s="7"/>
     </row>
@@ -1091,16 +1106,16 @@
         <v>44222.0</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28">
@@ -1108,16 +1123,16 @@
         <v>44223.0</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G28" s="33" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29">
@@ -1125,40 +1140,55 @@
         <v>44224.0</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G29" s="20" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="35"/>
+      <c r="A30" s="34">
+        <v>44225.0</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="G30" s="20" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="7" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34">
-      <c r="I34" s="36" t="s">
-        <v>71</v>
+      <c r="I34" s="35" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="50">
+  <mergeCells count="52">
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="G26:H26"/>
     <mergeCell ref="I34:K37"/>
     <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="G27:H27"/>
@@ -1166,6 +1196,7 @@
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="G28:H28"/>
     <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A11:C12"/>
     <mergeCell ref="D11:E12"/>

</xml_diff>

<commit_message>
Sprint backlog final version
</commit_message>
<xml_diff>
--- a/Sprint 1/Sprint_Backlog/Sprint backlog.xlsx
+++ b/Sprint 1/Sprint_Backlog/Sprint backlog.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="78">
   <si>
     <t>Agile Group 9 - Sprint 1</t>
   </si>
@@ -139,6 +139,9 @@
     <t>Shanna, Tim (database needs setup first)</t>
   </si>
   <si>
+    <t>N</t>
+  </si>
+  <si>
     <t>As a stakeholder, I want participants to only have access to questionnaires so that the rest of the experiment is private and safe</t>
   </si>
   <si>
@@ -237,7 +240,7 @@
     <t>example date</t>
   </si>
   <si>
-    <t>4 :)   3 :|   1 :(</t>
+    <t>M,B,S,I</t>
   </si>
   <si>
     <t>4 Spirits, 1 Mock, 2 Beer</t>
@@ -308,10 +311,10 @@
     <t>- Get all made pages working                                               - Get some basic SQL function to show off                                                                - Sprint Review</t>
   </si>
   <si>
-    <t>M,B,S,I</t>
-  </si>
-  <si>
     <t xml:space="preserve">daily scrum shouldn't cover the technicalities of work, it should focus on the next steps and help keep things moving - technicalities can be done at other times aside from the scrum </t>
+  </si>
+  <si>
+    <t>We expected to reach 11 completed story points, however there was a big delay in lawing down the fundamentals so stories only began properly taking form on day 2; though they can't be checked off as done yet</t>
   </si>
 </sst>
 </file>
@@ -504,7 +507,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -564,6 +567,9 @@
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
@@ -587,6 +593,9 @@
     </xf>
     <xf borderId="15" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -608,7 +617,36 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5734050" cy="3505200"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -972,214 +1010,222 @@
       <c r="H14" s="21">
         <v>2.0</v>
       </c>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
+      <c r="I14" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="J14" s="24"/>
     </row>
     <row r="15">
       <c r="A15" s="20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H15" s="21">
         <v>2.0</v>
       </c>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
+      <c r="I15" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="J15" s="24"/>
     </row>
     <row r="16">
       <c r="A16" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="24" t="s">
         <v>35</v>
       </c>
+      <c r="D16" s="25" t="s">
+        <v>36</v>
+      </c>
       <c r="F16" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H16" s="21">
         <v>2.0</v>
       </c>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
+      <c r="I16" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="J16" s="24"/>
     </row>
     <row r="17">
       <c r="A17" s="20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H17" s="21">
         <v>3.0</v>
       </c>
-      <c r="I17" s="23"/>
+      <c r="I17" s="23" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="25" t="s">
+      <c r="A18" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="F18" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
+      <c r="F18" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
     </row>
     <row r="19">
       <c r="I19" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="I20" s="27" t="s">
         <v>46</v>
+      </c>
+      <c r="I20" s="28" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="28" t="s">
-        <v>50</v>
+      <c r="A24" s="29" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="B25" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="30"/>
-      <c r="E25" s="29" t="s">
+      <c r="C25" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="F25" s="30"/>
-      <c r="G25" s="29" t="s">
+      <c r="D25" s="31"/>
+      <c r="E25" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="H25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="H25" s="32"/>
     </row>
     <row r="26">
       <c r="A26" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="7" t="s">
         <v>57</v>
       </c>
+      <c r="B26" s="33" t="s">
+        <v>58</v>
+      </c>
       <c r="C26" s="7"/>
     </row>
     <row r="27">
-      <c r="A27" s="32">
+      <c r="A27" s="34">
         <v>44222.0</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="32">
+      <c r="A28" s="34">
         <v>44223.0</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="G28" s="33" t="s">
         <v>65</v>
       </c>
+      <c r="G28" s="35" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" s="34">
+      <c r="A29" s="36">
         <v>44224.0</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G29" s="20" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="34">
+      <c r="A30" s="36">
         <v>44225.0</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G30" s="20" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="7" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="34">
-      <c r="I34" s="35" t="s">
+      <c r="I34" s="37" t="s">
         <v>76</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="F39" s="7" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>